<commit_message>
first test calibration data on servo instance, and it works whoooa:]
</commit_message>
<xml_diff>
--- a/kalkulator TIM PWM itp.xlsx
+++ b/kalkulator TIM PWM itp.xlsx
@@ -2067,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>